<commit_message>
finalized testing for Redis Chroma
</commit_message>
<xml_diff>
--- a/LLM Timing and Memory Tests.xlsx
+++ b/LLM Timing and Memory Tests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanw\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanw\Downloads\4300-rag-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1373227A-BCAC-43F6-B478-F359458BB107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA61633-91D9-434C-AA27-2FF35616940F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{BDE260DA-6967-4512-804D-0CB1EFD34F16}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>Faiss</t>
   </si>
   <si>
-    <t>Embedding Query Time (Seconds)</t>
-  </si>
-  <si>
     <t>LLM Response Time (Seconds)</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>3,2,3</t>
+  </si>
+  <si>
+    <t>Embedding Time (Seconds)</t>
   </si>
 </sst>
 </file>
@@ -181,7 +181,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A56B2A7-EF14-4BD9-B3C8-816356ACEDD1}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,25 +550,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -582,27 +582,27 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>1.2322</v>
+        <v>41.14</v>
       </c>
       <c r="E2">
-        <v>9.4745000000000008</v>
+        <v>20.93</v>
       </c>
       <c r="F2">
         <f>SUM(D2:E2)</f>
-        <v>10.706700000000001</v>
+        <v>62.07</v>
       </c>
       <c r="G2">
-        <v>0.1</v>
+        <v>5.71</v>
       </c>
       <c r="H2">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="I2">
         <f>SUM(G2:H2)</f>
-        <v>0.12000000000000001</v>
+        <v>5.72</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -616,27 +616,27 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>0.3906</v>
+        <v>137.69999999999999</v>
       </c>
       <c r="E3">
-        <v>29.507899999999999</v>
+        <v>11.14</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F19" si="0">SUM(D3:E3)</f>
-        <v>29.898499999999999</v>
+        <v>148.83999999999997</v>
       </c>
       <c r="G3">
-        <v>22.48</v>
+        <v>5.71</v>
       </c>
       <c r="H3">
-        <v>6.56</v>
+        <v>5.42</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I19" si="1">SUM(G3:H3)</f>
-        <v>29.04</v>
+        <v>11.129999999999999</v>
       </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -650,27 +650,27 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>2.6800999999999999</v>
+        <v>102.83</v>
       </c>
       <c r="E4">
-        <v>38.381599999999999</v>
+        <v>20.89</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>41.061700000000002</v>
+        <v>123.72</v>
       </c>
       <c r="G4">
-        <v>0.18</v>
+        <v>5.53</v>
       </c>
       <c r="H4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.03</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>5.5600000000000005</v>
       </c>
       <c r="K4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -684,27 +684,27 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>0.66569999999999996</v>
+        <v>41.23</v>
       </c>
       <c r="E5">
-        <v>29.314299999999999</v>
+        <v>30.41</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>29.98</v>
+        <v>71.64</v>
       </c>
       <c r="G5">
-        <v>0.01</v>
+        <v>5.71</v>
       </c>
       <c r="H5">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>5.7299999999999995</v>
       </c>
       <c r="K5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -718,27 +718,27 @@
         <v>8</v>
       </c>
       <c r="D6">
-        <v>0.1895</v>
+        <v>134.97999999999999</v>
       </c>
       <c r="E6">
-        <v>28.750800000000002</v>
+        <v>35.47</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>28.940300000000001</v>
+        <v>170.45</v>
       </c>
       <c r="G6">
-        <v>12.34</v>
+        <v>5.71</v>
       </c>
       <c r="H6">
-        <v>4.6500000000000004</v>
+        <v>19.059999999999999</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>16.990000000000002</v>
+        <v>24.77</v>
       </c>
       <c r="K6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -752,27 +752,27 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>3.0749</v>
+        <v>104.48</v>
       </c>
       <c r="E7">
-        <v>32.969099999999997</v>
+        <v>48.75</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>36.043999999999997</v>
+        <v>153.23000000000002</v>
       </c>
       <c r="G7">
-        <v>0.2</v>
+        <v>5.53</v>
       </c>
       <c r="H7">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>0.24000000000000002</v>
+        <v>5.58</v>
       </c>
       <c r="K7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -785,16 +785,28 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
+      <c r="D8">
+        <v>49.76</v>
+      </c>
+      <c r="E8">
+        <v>22.43</v>
+      </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72.19</v>
+      </c>
+      <c r="G8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H8">
+        <v>0.02</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="K8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -807,16 +819,28 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
+      <c r="D9">
+        <v>143.49</v>
+      </c>
+      <c r="E9">
+        <v>12.2</v>
+      </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>155.69</v>
+      </c>
+      <c r="G9">
+        <v>178.73</v>
+      </c>
+      <c r="H9">
+        <v>-111.61</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>67.11999999999999</v>
       </c>
       <c r="K9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -829,16 +853,28 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
+      <c r="D10">
+        <v>115.27</v>
+      </c>
+      <c r="E10">
+        <v>29.25</v>
+      </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>144.51999999999998</v>
+      </c>
+      <c r="G10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H10">
+        <v>0.77</v>
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.97</v>
       </c>
       <c r="K10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -851,16 +887,28 @@
       <c r="C11" t="s">
         <v>9</v>
       </c>
+      <c r="D11">
+        <v>49.87</v>
+      </c>
+      <c r="E11">
+        <v>35.69</v>
+      </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>85.56</v>
+      </c>
+      <c r="G11">
+        <v>0.61</v>
+      </c>
+      <c r="H11">
+        <v>0.79</v>
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -873,16 +921,28 @@
       <c r="C12" t="s">
         <v>9</v>
       </c>
+      <c r="D12">
+        <v>142.21</v>
+      </c>
+      <c r="E12">
+        <v>37.94</v>
+      </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>180.15</v>
+      </c>
+      <c r="G12">
+        <v>190.39</v>
+      </c>
+      <c r="H12">
+        <v>0.41</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>190.79999999999998</v>
       </c>
       <c r="K12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -895,16 +955,28 @@
       <c r="C13" t="s">
         <v>9</v>
       </c>
+      <c r="D13">
+        <v>112.32</v>
+      </c>
+      <c r="E13">
+        <v>38.450000000000003</v>
+      </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150.76999999999998</v>
+      </c>
+      <c r="G13">
+        <v>1.21</v>
+      </c>
+      <c r="H13">
+        <v>0.01</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.22</v>
       </c>
       <c r="K13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -926,7 +998,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -948,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -970,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -992,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1014,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1036,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>